<commit_message>
- Se realizó el testing de las historias: Recuperar Contraseña, Registrar Equipo y Modifica Campeonato
</commit_message>
<xml_diff>
--- a/Documentacion/Testing/Sprint 2/Registro Resultado Testing.xlsx
+++ b/Documentacion/Testing/Sprint 2/Registro Resultado Testing.xlsx
@@ -4,20 +4,27 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="TC_001" sheetId="1" r:id="rId1"/>
     <sheet name="TC_002" sheetId="2" r:id="rId2"/>
     <sheet name="TC_003" sheetId="3" r:id="rId3"/>
-    <sheet name="Defectos Conocidos" sheetId="4" r:id="rId4"/>
+    <sheet name="TC_004" sheetId="5" r:id="rId4"/>
+    <sheet name="TC_005" sheetId="6" r:id="rId5"/>
+    <sheet name="TC_006" sheetId="7" r:id="rId6"/>
+    <sheet name="TC_007" sheetId="8" r:id="rId7"/>
+    <sheet name="TC_008" sheetId="9" r:id="rId8"/>
+    <sheet name="TC_009" sheetId="10" r:id="rId9"/>
+    <sheet name="TC_010" sheetId="11" r:id="rId10"/>
+    <sheet name="Defectos Conocidos" sheetId="4" r:id="rId11"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="55">
   <si>
     <t>QUE GOLAZO!</t>
   </si>
@@ -158,6 +165,84 @@
   </si>
   <si>
     <t>3- Registrar Equipo</t>
+  </si>
+  <si>
+    <t>No está validado el teléfono. Sólo que sea numérico, pero puede ingresar "123" como teléfono válido</t>
+  </si>
+  <si>
+    <t>Pasó</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Se registró el equipo y su delegado correctamente</t>
+  </si>
+  <si>
+    <t>Se registró el equipo y sus delegados correctamente</t>
+  </si>
+  <si>
+    <t>No está validad que los colores de camiseta sean iguales</t>
+  </si>
+  <si>
+    <t>No me deja registrar un equipo ya registrado</t>
+  </si>
+  <si>
+    <t>TC_004</t>
+  </si>
+  <si>
+    <t>No me registra el equipo y me solicita ingresar al menos un delegado</t>
+  </si>
+  <si>
+    <t>TC_005</t>
+  </si>
+  <si>
+    <t>No me registra el equipo y me informa que hasta dos delegados puedo ingresar</t>
+  </si>
+  <si>
+    <t>TC_006</t>
+  </si>
+  <si>
+    <t>No me registra el equipo y me informa que los delegados no pueden tener igual nombre</t>
+  </si>
+  <si>
+    <t>Cuando ingreso un delegado con el mismo nombre debería dejarme editarlo no borrar todos los datos</t>
+  </si>
+  <si>
+    <t>TC_007</t>
+  </si>
+  <si>
+    <t>Florencia Rojas</t>
+  </si>
+  <si>
+    <t>Me recupera correctamente la contraseña</t>
+  </si>
+  <si>
+    <t>Error cosmético: cuando pongo recuperar la contraseña, me sugiere una contraseña.</t>
+  </si>
+  <si>
+    <t>Me informa que no hay ningún usuario registrado con el mail incorrecto</t>
+  </si>
+  <si>
+    <t>TC_008</t>
+  </si>
+  <si>
+    <t>TC_009</t>
+  </si>
+  <si>
+    <t>Me modifica correctamente el campeonato</t>
+  </si>
+  <si>
+    <t>TC_010</t>
+  </si>
+  <si>
+    <t>Error Cosmético: en la ventana modal de modificar el titulo es "Registrar Nuevo Torneo"</t>
+  </si>
+  <si>
+    <t>Pendiente de Corrección</t>
+  </si>
+  <si>
+    <t>No me deja modificar el nombre porque ya existe ese nombre para ese usuario</t>
   </si>
 </sst>
 </file>
@@ -193,7 +278,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -209,6 +294,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00CC00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -240,7 +337,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -264,6 +361,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -276,12 +376,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF00CC00"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -583,14 +705,14 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.5703125" customWidth="1"/>
-    <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" customWidth="1"/>
     <col min="4" max="4" width="21.140625" customWidth="1"/>
     <col min="5" max="5" width="18.7109375" customWidth="1"/>
     <col min="6" max="6" width="16.28515625" customWidth="1"/>
@@ -600,43 +722,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
     </row>
     <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -667,23 +789,37 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
+      <c r="B5" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="20">
+        <v>41837</v>
+      </c>
+      <c r="I5" s="1">
+        <v>85</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -694,9 +830,7 @@
       <c r="I6" s="1"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -767,64 +901,65 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="D9" sqref="D8:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" customWidth="1"/>
-    <col min="5" max="5" width="29" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="3" max="4" width="15.85546875" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" customWidth="1"/>
+    <col min="6" max="6" width="27.7109375" customWidth="1"/>
+    <col min="7" max="7" width="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-    </row>
-    <row r="4" spans="1:9" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A3" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+    </row>
+    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -852,23 +987,37 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
+        <v>51</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="H5" s="20">
+        <v>41837</v>
+      </c>
+      <c r="I5" s="1">
+        <v>85</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -879,9 +1028,7 @@
       <c r="I6" s="1"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -902,6 +1049,9 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:I1"/>
@@ -912,157 +1062,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" customWidth="1"/>
-    <col min="5" max="5" width="40.140625" customWidth="1"/>
-    <col min="6" max="6" width="22" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-    </row>
-    <row r="4" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-    </row>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="A3:I3"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1080,11 +1085,11 @@
       <c r="A1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
       <c r="E1" s="8" t="s">
         <v>24</v>
       </c>
@@ -1099,11 +1104,11 @@
       <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
       <c r="E2" s="7" t="s">
         <v>28</v>
       </c>
@@ -1114,259 +1119,290 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
+    <row r="3" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
+        <v>2</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
+      <c r="A4" s="7">
+        <v>3</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
+      <c r="A5" s="7">
+        <v>4</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
       <c r="E13" s="9"/>
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
       <c r="G15" s="9"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
       <c r="E16" s="9"/>
       <c r="F16" s="9"/>
       <c r="G16" s="9"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
       <c r="G18" s="9"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
       <c r="E19" s="9"/>
       <c r="F19" s="9"/>
       <c r="G19" s="9"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
-      <c r="B22" s="12"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
-      <c r="B23" s="12"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
       <c r="E23" s="9"/>
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
-      <c r="B24" s="12"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
-      <c r="B25" s="12"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
       <c r="E25" s="9"/>
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="7"/>
-      <c r="B26" s="12"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
       <c r="E26" s="9"/>
       <c r="F26" s="9"/>
       <c r="G26" s="9"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
-      <c r="B27" s="12"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
       <c r="E27" s="9"/>
       <c r="F27" s="9"/>
       <c r="G27" s="9"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="12"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
       <c r="E28" s="9"/>
       <c r="F28" s="9"/>
       <c r="G28" s="9"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
-      <c r="B29" s="12"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
       <c r="E29" s="9"/>
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B5:D5"/>
     <mergeCell ref="B21:D21"/>
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="B11:D11"/>
@@ -1379,15 +1415,1296 @@
     <mergeCell ref="B18:D18"/>
     <mergeCell ref="B19:D19"/>
     <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B27:D27"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" customWidth="1"/>
+    <col min="5" max="5" width="29" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+    </row>
+    <row r="4" spans="1:9" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="20">
+        <v>41837</v>
+      </c>
+      <c r="I5" s="1">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A3:I3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="24.28515625" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" customWidth="1"/>
+    <col min="5" max="5" width="40.140625" customWidth="1"/>
+    <col min="6" max="6" width="22" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+    </row>
+    <row r="4" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="20">
+        <v>41837</v>
+      </c>
+      <c r="I5" s="1">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A3:I3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I10" sqref="A1:I10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="3" max="4" width="15.85546875" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" customWidth="1"/>
+    <col min="7" max="7" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+    </row>
+    <row r="4" spans="1:9" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="20">
+        <v>41837</v>
+      </c>
+      <c r="I5" s="1">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A3:I3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I11" sqref="A1:I11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="3" max="4" width="15.85546875" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" customWidth="1"/>
+    <col min="7" max="7" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+    </row>
+    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="20">
+        <v>41837</v>
+      </c>
+      <c r="I5" s="1">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A3:I3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J10" sqref="A1:J10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="3" max="4" width="15.85546875" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" customWidth="1"/>
+    <col min="7" max="7" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+    </row>
+    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="20">
+        <v>41837</v>
+      </c>
+      <c r="I5" s="1">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A3:I3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="3" max="4" width="15.85546875" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" customWidth="1"/>
+    <col min="6" max="6" width="27.7109375" customWidth="1"/>
+    <col min="7" max="7" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+    </row>
+    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="H5" s="20">
+        <v>41837</v>
+      </c>
+      <c r="I5" s="1">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A3:I3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J11" sqref="A1:J11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="3" max="4" width="15.85546875" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" customWidth="1"/>
+    <col min="6" max="6" width="27.7109375" customWidth="1"/>
+    <col min="7" max="7" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+    </row>
+    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="20">
+        <v>41837</v>
+      </c>
+      <c r="I5" s="1">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A3:I3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="3" max="4" width="15.85546875" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" customWidth="1"/>
+    <col min="6" max="6" width="27.7109375" customWidth="1"/>
+    <col min="7" max="7" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+    </row>
+    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="H5" s="20">
+        <v>41837</v>
+      </c>
+      <c r="I5" s="1">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
- Presentación Grado de Avances
</commit_message>
<xml_diff>
--- a/Documentacion/Testing/Sprint 2/Registro Resultado Testing.xlsx
+++ b/Documentacion/Testing/Sprint 2/Registro Resultado Testing.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="3" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="TC_001" sheetId="1" r:id="rId1"/>
@@ -158,9 +158,6 @@
     <t>Cuando la Imagen cargada tiene formato incorrecto, en la modificación del equipo, le debe  permitir registrarla nuevamente</t>
   </si>
   <si>
-    <t>Pendiente</t>
-  </si>
-  <si>
     <t>Paula Pedrosa</t>
   </si>
   <si>
@@ -243,6 +240,9 @@
   </si>
   <si>
     <t>No me deja modificar el nombre porque ya existe ese nombre para ese usuario</t>
+  </si>
+  <si>
+    <t>Corregido</t>
   </si>
 </sst>
 </file>
@@ -361,6 +361,20 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -376,22 +390,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -722,43 +722,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
     </row>
     <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -793,25 +793,25 @@
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="21" t="s">
+      <c r="B5" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="F5" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H5" s="20">
+        <v>30</v>
+      </c>
+      <c r="H5" s="14">
         <v>41837</v>
       </c>
       <c r="I5" s="1">
@@ -920,43 +920,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
     </row>
     <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
@@ -989,27 +989,27 @@
     </row>
     <row r="5" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="B5" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="C5" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="D5" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F5" s="22" t="s">
+      <c r="G5" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="G5" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="H5" s="20">
+      <c r="H5" s="14">
         <v>41837</v>
       </c>
       <c r="I5" s="1">
@@ -1066,8 +1066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1085,11 +1085,11 @@
       <c r="A1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
       <c r="E1" s="8" t="s">
         <v>24</v>
       </c>
@@ -1104,305 +1104,304 @@
       <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
       <c r="E2" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F2" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>26</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>2</v>
       </c>
-      <c r="B3" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
+      <c r="B3" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
       <c r="E3" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>26</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>3</v>
       </c>
-      <c r="B4" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
+      <c r="B4" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
       <c r="E4" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F4" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="G4" s="7" t="s">
         <v>26</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>4</v>
       </c>
-      <c r="B5" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
+      <c r="B5" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
       <c r="E5" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F5" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="G5" s="7" t="s">
         <v>26</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
       <c r="E13" s="9"/>
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
       <c r="G15" s="9"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
       <c r="E16" s="9"/>
       <c r="F16" s="9"/>
       <c r="G16" s="9"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
       <c r="G18" s="9"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
       <c r="E19" s="9"/>
       <c r="F19" s="9"/>
       <c r="G19" s="9"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
       <c r="E23" s="9"/>
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
-      <c r="B25" s="13"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
       <c r="E25" s="9"/>
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="7"/>
-      <c r="B26" s="13"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="19"/>
       <c r="E26" s="9"/>
       <c r="F26" s="9"/>
       <c r="G26" s="9"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
-      <c r="B27" s="13"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
+      <c r="B27" s="19"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
       <c r="E27" s="9"/>
       <c r="F27" s="9"/>
       <c r="G27" s="9"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
-      <c r="B28" s="13"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
       <c r="E28" s="9"/>
       <c r="F28" s="9"/>
       <c r="G28" s="9"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
-      <c r="B29" s="13"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
+      <c r="B29" s="19"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
       <c r="E29" s="9"/>
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B27:D27"/>
     <mergeCell ref="B21:D21"/>
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="B11:D11"/>
@@ -1415,14 +1414,15 @@
     <mergeCell ref="B18:D18"/>
     <mergeCell ref="B19:D19"/>
     <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B5:D5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1448,43 +1448,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
     </row>
     <row r="4" spans="1:9" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
@@ -1519,25 +1519,25 @@
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="19" t="s">
-        <v>33</v>
+      <c r="B5" s="13" t="s">
+        <v>32</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="F5" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H5" s="20">
+        <v>30</v>
+      </c>
+      <c r="H5" s="14">
         <v>41837</v>
       </c>
       <c r="I5" s="1">
@@ -1605,43 +1605,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
     </row>
     <row r="4" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
@@ -1676,25 +1676,25 @@
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="19" t="s">
-        <v>35</v>
+      <c r="B5" s="13" t="s">
+        <v>34</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="F5" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H5" s="20">
+        <v>30</v>
+      </c>
+      <c r="H5" s="14">
         <v>41837</v>
       </c>
       <c r="I5" s="1">
@@ -1763,43 +1763,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
     </row>
     <row r="4" spans="1:9" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
@@ -1832,27 +1832,27 @@
     </row>
     <row r="5" spans="1:9" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="21" t="s">
+      <c r="C5" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="F5" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H5" s="20">
+        <v>30</v>
+      </c>
+      <c r="H5" s="14">
         <v>41837</v>
       </c>
       <c r="I5" s="1">
@@ -1924,43 +1924,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
     </row>
     <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
@@ -1993,27 +1993,27 @@
     </row>
     <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="21" t="s">
+      <c r="C5" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="F5" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H5" s="20">
+        <v>30</v>
+      </c>
+      <c r="H5" s="14">
         <v>41837</v>
       </c>
       <c r="I5" s="1">
@@ -2085,43 +2085,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
     </row>
     <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
@@ -2154,27 +2154,27 @@
     </row>
     <row r="5" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="21" t="s">
+      <c r="C5" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="F5" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H5" s="20">
+        <v>30</v>
+      </c>
+      <c r="H5" s="14">
         <v>41837</v>
       </c>
       <c r="I5" s="1">
@@ -2231,7 +2231,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -2246,43 +2246,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
     </row>
     <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
@@ -2315,27 +2315,27 @@
     </row>
     <row r="5" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="D5" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="C5" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="D5" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F5" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="G5" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="H5" s="20">
+      <c r="G5" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="H5" s="14">
         <v>41837</v>
       </c>
       <c r="I5" s="1">
@@ -2407,43 +2407,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
     </row>
     <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
@@ -2476,27 +2476,27 @@
     </row>
     <row r="5" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B5" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="C5" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="D5" s="21" t="s">
+      <c r="B5" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F5" s="22" t="s">
-        <v>46</v>
+      <c r="F5" s="16" t="s">
+        <v>45</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H5" s="20">
+        <v>30</v>
+      </c>
+      <c r="H5" s="14">
         <v>41837</v>
       </c>
       <c r="I5" s="1">
@@ -2568,43 +2568,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
     </row>
     <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
@@ -2637,27 +2637,27 @@
     </row>
     <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="D5" s="21" t="s">
+      <c r="C5" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F5" s="22" t="s">
+      <c r="F5" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="G5" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="G5" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="H5" s="20">
+      <c r="H5" s="14">
         <v>41837</v>
       </c>
       <c r="I5" s="1">

</xml_diff>